<commit_message>
parei em learning rate 0,01
</commit_message>
<xml_diff>
--- a/Project/Phase III/Resultados.xlsx
+++ b/Project/Phase III/Resultados.xlsx
@@ -1179,8 +1179,12 @@
         <v>0.01</v>
       </c>
       <c r="F15" s="4"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="6"/>
+      <c r="G15" s="5">
+        <v>26.345199999999998</v>
+      </c>
+      <c r="H15" s="6">
+        <v>1420.1068</v>
+      </c>
     </row>
     <row r="16" ht="39.950000000000003" customHeight="1">
       <c r="A16" s="10" t="s">

</xml_diff>

<commit_message>
relatório só falta diagrama
</commit_message>
<xml_diff>
--- a/Project/Phase III/Resultados.xlsx
+++ b/Project/Phase III/Resultados.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Deep" sheetId="1" state="visible" r:id="rId1"/>
@@ -1426,7 +1426,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="100" workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="I37" activeCellId="0" sqref="I37"/>
     </sheetView>
   </sheetViews>
@@ -1480,8 +1480,12 @@
         <v>0.001</v>
       </c>
       <c r="F3" s="4"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="6"/>
+      <c r="G3" s="5">
+        <v>42.4221</v>
+      </c>
+      <c r="H3" s="6">
+        <v>8208.0458999999992</v>
+      </c>
     </row>
     <row r="4" ht="15.949999999999999" customHeight="1"/>
     <row r="5" ht="16.5"/>
@@ -1521,141 +1525,126 @@
         <v>4505.3271000000004</v>
       </c>
     </row>
-    <row r="8" ht="39.950000000000003" customHeight="1">
-      <c r="A8" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="11">
-        <v>2</v>
-      </c>
-      <c r="C8" s="11">
-        <v>32</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="4">
-        <v>0.001</v>
-      </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="6"/>
-    </row>
-    <row r="9" ht="39.950000000000003" customHeight="1">
-      <c r="A9" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="11">
-        <v>4</v>
-      </c>
-      <c r="C9" s="11">
-        <v>32</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="4">
-        <v>0.001</v>
-      </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="6"/>
+    <row r="8" ht="16.5">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" ht="56.100000000000001" customHeight="1">
+      <c r="A9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="9"/>
     </row>
     <row r="10" ht="39.950000000000003" customHeight="1">
       <c r="A10" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="11">
-        <v>6</v>
-      </c>
-      <c r="C10" s="12">
+        <v>9</v>
+      </c>
+      <c r="B10" s="13">
+        <v>4</v>
+      </c>
+      <c r="C10" s="4">
         <v>32</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="4">
-        <v>0.001</v>
+      <c r="E10" s="11">
+        <v>0.0001</v>
       </c>
       <c r="F10" s="4"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="6"/>
+      <c r="G10" s="5">
+        <v>502.60969999999998</v>
+      </c>
+      <c r="H10" s="6">
+        <v>881962.875</v>
+      </c>
     </row>
     <row r="11" ht="39.950000000000003" customHeight="1">
       <c r="A11" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="11">
-        <v>6</v>
-      </c>
-      <c r="C11" s="12">
-        <v>256</v>
+        <v>10</v>
+      </c>
+      <c r="B11" s="13">
+        <v>4</v>
+      </c>
+      <c r="C11" s="4">
+        <v>32</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="4">
-        <v>0.001</v>
+      <c r="E11" s="11">
+        <v>0.01</v>
       </c>
       <c r="F11" s="4"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="6"/>
-    </row>
-    <row r="13" ht="56.100000000000001" customHeight="1">
-      <c r="A13" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="9"/>
-    </row>
-    <row r="14" ht="39.950000000000003" customHeight="1">
-      <c r="A14" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="13">
+      <c r="G11" s="5">
+        <v>48753.675799999997</v>
+      </c>
+      <c r="H11" s="6">
+        <v>2473905408</v>
+      </c>
+    </row>
+    <row r="12" ht="39.950000000000003" customHeight="1">
+      <c r="A12" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="13">
         <v>4</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C12" s="4">
         <v>32</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="11">
-        <v>0.0001</v>
-      </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="6"/>
-    </row>
-    <row r="15" ht="39.950000000000003" customHeight="1">
-      <c r="A15" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="13">
-        <v>4</v>
-      </c>
-      <c r="C15" s="4">
-        <v>32</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="11">
-        <v>0.01</v>
-      </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="6"/>
+      <c r="E12" s="11">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="5">
+        <v>55.784199999999998</v>
+      </c>
+      <c r="H12" s="6">
+        <v>4161.8584000000001</v>
+      </c>
+    </row>
+    <row r="13" ht="16.5">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" ht="16.5"/>
+    <row r="15" ht="56.100000000000001" customHeight="1">
+      <c r="A15" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="9"/>
     </row>
     <row r="16" ht="39.950000000000003" customHeight="1">
       <c r="A16" s="10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B16" s="13">
         <v>4</v>
@@ -1663,15 +1652,19 @@
       <c r="C16" s="4">
         <v>32</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="11">
-        <v>0.10000000000000001</v>
+      <c r="D16" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0.001</v>
       </c>
       <c r="F16" s="4"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="6"/>
+      <c r="G16" s="5">
+        <v>48752.667999999998</v>
+      </c>
+      <c r="H16" s="6">
+        <v>2473807104</v>
+      </c>
     </row>
     <row r="17" ht="39.950000000000003" customHeight="1">
       <c r="A17" s="10" t="s">
@@ -1683,88 +1676,79 @@
       <c r="C17" s="4">
         <v>32</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="12">
-        <v>1</v>
+      <c r="D17" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0.001</v>
       </c>
       <c r="F17" s="4"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="6"/>
-    </row>
-    <row r="18" ht="39.950000000000003" customHeight="1">
-      <c r="A18" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="13">
-        <v>4</v>
-      </c>
-      <c r="C18" s="4">
-        <v>32</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="12">
-        <v>2</v>
-      </c>
-      <c r="F18" s="4"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="6"/>
-    </row>
-    <row r="20" ht="16.5"/>
-    <row r="21" ht="56.100000000000001" customHeight="1">
-      <c r="A21" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="9"/>
-    </row>
-    <row r="22" ht="39.950000000000003" customHeight="1">
-      <c r="A22" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="13">
-        <v>4</v>
-      </c>
-      <c r="C22" s="4">
-        <v>32</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" s="4">
-        <v>0.001</v>
-      </c>
-      <c r="F22" s="4"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="6"/>
-    </row>
-    <row r="23" ht="39.950000000000003" customHeight="1">
-      <c r="A23" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23" s="13">
-        <v>4</v>
-      </c>
-      <c r="C23" s="4">
-        <v>32</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" s="4">
-        <v>0.001</v>
-      </c>
-      <c r="F23" s="4"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="6"/>
+      <c r="G17" s="5">
+        <v>48752.667999999998</v>
+      </c>
+      <c r="H17" s="6">
+        <v>2473807104</v>
+      </c>
+    </row>
+    <row r="18" ht="16.5">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" ht="16.5">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" ht="16.5">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" ht="16.5">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" ht="16.5">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" ht="16.5">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
     </row>
     <row r="24" ht="16.5">
       <c r="A24" s="1"/>
@@ -1786,71 +1770,11 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" ht="16.5">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-    </row>
-    <row r="27" ht="16.5">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-    </row>
-    <row r="28" ht="16.5">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-    </row>
-    <row r="29" ht="16.5">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-    </row>
-    <row r="30" ht="16.5">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-    </row>
-    <row r="31" ht="16.5">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A6:H6"/>
-    <mergeCell ref="A13:H13"/>
-    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A15:H15"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>